<commit_message>
login node Stateless service
</commit_message>
<xml_diff>
--- a/bin/config/xlsx/tip/Tip.xlsx
+++ b/bin/config/xlsx/tip/Tip.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="192">
   <si>
     <t>name</t>
   </si>
@@ -276,6 +276,24 @@
   </si>
   <si>
     <t xml:space="preserve">   LoginRedisSetFailed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    TooManyDevices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LoginFSMLoadFailed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LoginFSMEventFailed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LoginAccountDataLoadFaile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LoginSessionNotFound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LoginAccountDataLoadFailed</t>
   </si>
   <si>
     <t>//scene_error</t>
@@ -1277,13 +1295,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1544,10 +1555,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:B155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1900,75 +1911,75 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" ht="20" customHeight="1" spans="1:1">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" ht="20" customHeight="1" spans="1:2">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>83</v>
       </c>
-      <c r="B64" t="s">
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" ht="20" customHeight="1" spans="1:1">
-      <c r="A65" t="s">
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
         <v>86</v>
       </c>
-      <c r="B66" t="s">
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+    <row r="69" ht="20" customHeight="1" spans="1:1">
+      <c r="A69" t="s">
         <v>88</v>
       </c>
-      <c r="B67" t="s">
+    </row>
+    <row r="70" ht="20" customHeight="1" spans="1:2">
+      <c r="A70" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
+      <c r="B70" t="s">
         <v>90</v>
       </c>
-      <c r="B68" t="s">
+    </row>
+    <row r="71" ht="20" customHeight="1" spans="1:1">
+      <c r="A71" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
+      <c r="B72" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
+      <c r="B73" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
+      <c r="B74" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2257,133 +2268,163 @@
         <v>154</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:1">
       <c r="A132" t="s">
         <v>155</v>
       </c>
-      <c r="B132" t="s">
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
-      <c r="A133" t="s">
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
         <v>157</v>
       </c>
-      <c r="B133" t="s">
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
-      <c r="A134" t="s">
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
         <v>159</v>
       </c>
-      <c r="B134" t="s">
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" t="s">
-        <v>161</v>
-      </c>
-      <c r="B135" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" t="s">
-        <v>163</v>
-      </c>
-      <c r="B136" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" t="s">
-        <v>165</v>
-      </c>
-      <c r="B137" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B138" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>169</v>
+        <v>163</v>
+      </c>
+      <c r="B139" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B140" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B141" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>174</v>
+        <v>169</v>
+      </c>
+      <c r="B142" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
+        <v>171</v>
+      </c>
+      <c r="B143" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>173</v>
+      </c>
+      <c r="B144" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
         <v>175</v>
       </c>
-      <c r="B143" t="s">
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
-      <c r="A144" t="s">
+      <c r="B146" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" t="s">
-        <v>178</v>
-      </c>
-      <c r="B145" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1">
-      <c r="A146" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B147" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
+        <v>181</v>
+      </c>
+      <c r="B149" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
         <v>184</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B151" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>187</v>
+      </c>
+      <c r="B153" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>190</v>
+      </c>
+      <c r="B155" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>